<commit_message>
R. padi genomic reads info added
</commit_message>
<xml_diff>
--- a/Data_Summary_APHID_RNASEQ.xlsx
+++ b/Data_Summary_APHID_RNASEQ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="206">
   <si>
     <t>Sample Description</t>
   </si>
@@ -736,6 +736,45 @@
   </si>
   <si>
     <t>LDI4461</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>Reads</t>
+  </si>
+  <si>
+    <t>R1 mean Q30 to base</t>
+  </si>
+  <si>
+    <t>R2 mean Q30 to base</t>
+  </si>
+  <si>
+    <t>Sample Alias</t>
+  </si>
+  <si>
+    <t>Mean insert size less adaptors</t>
+  </si>
+  <si>
+    <t>Run Alias</t>
+  </si>
+  <si>
+    <t>1566_LIB18620_LDI16209_NoIndex_L002_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>PRO973_S3_gDNA</t>
+  </si>
+  <si>
+    <t>LIB18620</t>
+  </si>
+  <si>
+    <t>LDI16209</t>
+  </si>
+  <si>
+    <t>150825_SN790_0030_BH77HYBCXX</t>
+  </si>
+  <si>
+    <t>R. padi GENOME read</t>
   </si>
 </sst>
 </file>
@@ -933,7 +972,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1113,6 +1152,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1274,7 +1319,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1315,6 +1360,8 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1657,10 +1704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="58.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3780,18 +3827,95 @@
       <c r="S32" s="8"/>
       <c r="T32" s="8"/>
     </row>
-    <row r="33" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>151</v>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B38" s="18">
+        <v>161482796</v>
+      </c>
+      <c r="C38">
+        <v>219</v>
+      </c>
+      <c r="D38">
+        <v>189</v>
+      </c>
+      <c r="E38" t="s">
+        <v>201</v>
+      </c>
+      <c r="F38" t="s">
+        <v>99</v>
+      </c>
+      <c r="G38" t="s">
+        <v>202</v>
+      </c>
+      <c r="H38" t="s">
+        <v>203</v>
+      </c>
+      <c r="I38" t="s">
+        <v>35</v>
+      </c>
+      <c r="J38">
+        <v>405</v>
+      </c>
+      <c r="K38" t="s">
+        <v>204</v>
+      </c>
+      <c r="L38">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>